<commit_message>
Fixed excel file example with last patches.
</commit_message>
<xml_diff>
--- a/examples/example.xlsx
+++ b/examples/example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Affichage" sheetId="1" state="visible" r:id="rId2"/>
@@ -101,7 +101,7 @@
     <t xml:space="preserve">Introduction à la physique expérimentale</t>
   </si>
   <si>
-    <t xml:space="preserve">PHY2701</t>
+    <t xml:space="preserve">PHY2710</t>
   </si>
   <si>
     <t xml:space="preserve">Astronomie et astrophysique</t>
@@ -161,31 +161,31 @@
     <t xml:space="preserve">Alice A</t>
   </si>
   <si>
-    <t xml:space="preserve">1441-30, 1620-30, 1620-30, 1620-90, 1620-90, 1651-30</t>
+    <t xml:space="preserve">PHY1441-30, PHY1620-30, PHY1620-30, PHY1620-90, PHY1620-90, PHY1651-30</t>
   </si>
   <si>
     <t xml:space="preserve">Matière Condensée</t>
   </si>
   <si>
-    <t xml:space="preserve">1441-90, 1620-90</t>
+    <t xml:space="preserve">PHY1441-90, PHY1620-90</t>
   </si>
   <si>
     <t xml:space="preserve">Bob B</t>
   </si>
   <si>
-    <t xml:space="preserve">1441-30, 2701, 2701, 2701, 2701, 2701</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1441-90, 2710</t>
+    <t xml:space="preserve">PHY1441-30, PHY2701, PHY2701, PHY2701, PHY2701, PHY2701</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHY1441-90, PHY2710</t>
   </si>
   <si>
     <t xml:space="preserve">Charlie C</t>
   </si>
   <si>
-    <t xml:space="preserve">2710, 2710, 2400, 2400</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2710, 2400</t>
+    <t xml:space="preserve">PHY2710, PHY2710, PHY2400, PHY2400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHY2710, PHY2400</t>
   </si>
 </sst>
 </file>
@@ -195,7 +195,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -219,79 +219,6 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
@@ -299,7 +226,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -308,48 +235,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF000000"/>
         <bgColor rgb="FF003300"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -357,23 +248,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -397,54 +273,6 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -455,7 +283,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -467,95 +295,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -566,17 +318,17 @@
   </sheetPr>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.27"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="1" width="11.58"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="35.1530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.780612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="11.5816326530612"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -806,7 +558,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -821,21 +573,21 @@
   </sheetPr>
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K39" activeCellId="0" sqref="K39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.65"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="47.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.03"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="11.58"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.92857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.5816326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="5.6530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="68.9336734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.5816326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.234693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.5816326530612"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="11.5816326530612"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -945,7 +697,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
adding 1 equality in example excel file
</commit_message>
<xml_diff>
--- a/examples/example.xlsx
+++ b/examples/example.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
   <si>
     <t xml:space="preserve">Sigle</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t xml:space="preserve">PHY2710, PHY2400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denise D</t>
   </si>
 </sst>
 </file>
@@ -325,9 +328,9 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.5816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="35.1530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="35.4285714285714"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.780612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.6836734693878"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="11.5816326530612"/>
   </cols>
   <sheetData>
@@ -571,10 +574,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K39" activeCellId="0" sqref="K39"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -582,9 +585,9 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.92857142857143"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.5816326530612"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="5.6530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="68.9336734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="69.6173469387755"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.5816326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.234693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.3673469387755"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.5816326530612"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.030612244898"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="11.5816326530612"/>
@@ -691,6 +694,32 @@
         <v>3.42</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>3.42</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>